<commit_message>
Fix multi-currency imports (#94)
</commit_message>
<xml_diff>
--- a/tests/0000_00_00_import_configs_test.xlsx
+++ b/tests/0000_00_00_import_configs_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coreyvarma/investbrain/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79F7FB8-A2CD-0E4C-8C4F-E2A59123E1C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D044BE82-94CC-704A-AF91-E77CB7ADC8F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>Annotation</t>
   </si>
   <si>
-    <t>9cf8a662-7347-49fb-b9de-0cc1430a8d1f</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -100,7 +97,10 @@
     <t>Value</t>
   </si>
   <si>
-    <t>reinvest_dividends</t>
+    <t>[{"portfolio_id": "9e792bb8-94e7-4ed3-b8cc-43b50d34c337", "symbol": "ACME"}]</t>
+  </si>
+  <si>
+    <t>reinvested_dividends</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
         <v>12</v>
@@ -625,7 +625,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -635,18 +635,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>